<commit_message>
puxa facil carregado tudo, só falta criar um novo encaminhamento exclsivo telefeed
</commit_message>
<xml_diff>
--- a/horarios auto post.xlsx
+++ b/horarios auto post.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>Dia</t>
   </si>
@@ -62,9 +62,6 @@
     <t>X (02h)</t>
   </si>
   <si>
-    <t>Cyborg (01h)</t>
-  </si>
-  <si>
     <t>X (01h)</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>Net (12h)</t>
+  </si>
+  <si>
+    <t>PuxaFacil (01h)</t>
   </si>
 </sst>
 </file>
@@ -586,7 +586,7 @@
   <dimension ref="A2:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,19 +597,19 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -633,7 +633,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -648,7 +648,7 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="11" t="s">
@@ -661,7 +661,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -688,9 +688,11 @@
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="13" t="s">
+        <v>12</v>
+      </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="11"/>

</xml_diff>